<commit_message>
vault backup: 2025-06-20 09:00:18
</commit_message>
<xml_diff>
--- a/办公/五月份/第五周/报表数据整理20250529.xlsx
+++ b/办公/五月份/第五周/报表数据整理20250529.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22192" windowHeight="11175" tabRatio="814"/>
+    <workbookView windowWidth="22192" windowHeight="9855" tabRatio="814"/>
   </bookViews>
   <sheets>
     <sheet name="查询异议" sheetId="1" r:id="rId1"/>
@@ -1476,6 +1476,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1729,7 +1736,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1923,13 +1930,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="21" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="21" t="s">

</xml_diff>